<commit_message>
chore: update template_barang.xlsx content
</commit_message>
<xml_diff>
--- a/public/template_excel/template_barang.xlsx
+++ b/public/template_excel/template_barang.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kuliah (Lokal)\Semester 4\PWL\week-8\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\PWL_POS\public\template_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C73D82A6-7D98-4EF0-9766-BD8FE4759BD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F618764E-52C8-4007-8238-81F4BE171BBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{C3CA63BE-8197-439D-A899-0CE1C988BD00}"/>
   </bookViews>
@@ -447,7 +447,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -546,7 +546,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B6" t="s">
         <v>13</v>

</xml_diff>